<commit_message>
Some update on Coverage form of Burkina Faso.
</commit_message>
<xml_diff>
--- a/Coverage Survey/Burkina Faso/IVM+ALB/cs2_couverture.xlsx
+++ b/Coverage Survey/Burkina Faso/IVM+ALB/cs2_couverture.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="665" uniqueCount="417">
   <si>
     <t>form_title</t>
   </si>
@@ -1006,9 +1006,6 @@
     <t>volet_pas_aime</t>
   </si>
   <si>
-    <t>select_one volet_pas_aime</t>
-  </si>
-  <si>
     <t>1. Une fois par jour</t>
   </si>
   <si>
@@ -1222,9 +1219,6 @@
     <t>. &gt;=0 and . &lt;= 30</t>
   </si>
   <si>
-    <t>. &gt;=0 and . &lt;= 36</t>
-  </si>
-  <si>
     <t>selected(${IVM_ALB_recu},'Oui')</t>
   </si>
   <si>
@@ -1262,6 +1256,30 @@
   </si>
   <si>
     <t>string</t>
+  </si>
+  <si>
+    <t>Numéro du ménage</t>
+  </si>
+  <si>
+    <t>numero_Menage</t>
+  </si>
+  <si>
+    <t>. &gt;=0 and . &lt;= 11</t>
+  </si>
+  <si>
+    <t>8. Moins de 5 ans</t>
+  </si>
+  <si>
+    <t>Moins.de.5.ans</t>
+  </si>
+  <si>
+    <t>select_multiple volet_pas_aime</t>
+  </si>
+  <si>
+    <t>regex(.,'^[a-zA-Z]{1}[0-9]{2,3}$')</t>
+  </si>
+  <si>
+    <t>Le code doit contenir une lettre et deux chiffres chiffres</t>
   </si>
 </sst>
 </file>
@@ -1769,11 +1787,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K56"/>
+  <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A53" sqref="A53:XFD53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1831,7 +1849,7 @@
         <v>84</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D2" s="17"/>
       <c r="E2" s="12"/>
@@ -1839,7 +1857,7 @@
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
       <c r="I2" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J2" s="12"/>
     </row>
@@ -1859,12 +1877,12 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>25</v>
@@ -1875,752 +1893,759 @@
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="8" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>393</v>
-      </c>
-      <c r="B5" t="s">
+        <v>408</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>410</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="8" t="s">
+        <v>415</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>416</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>392</v>
+      </c>
+      <c r="B6" t="s">
         <v>136</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="I5" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="I6" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B7" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="H6" s="6"/>
-      <c r="I6" s="17" t="s">
-        <v>387</v>
-      </c>
-      <c r="J6" s="24"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>374</v>
-      </c>
-      <c r="C7" s="23" t="s">
-        <v>385</v>
-      </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="6"/>
       <c r="F7" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="8" t="s">
-        <v>86</v>
-      </c>
+        <v>394</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="6"/>
       <c r="I7" s="17" t="s">
-        <v>387</v>
-      </c>
-      <c r="J7" s="7"/>
+        <v>386</v>
+      </c>
+      <c r="J7" s="24"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>29</v>
+        <v>118</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>373</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>384</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="8" t="s">
+        <v>411</v>
+      </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="8" t="s">
+        <v>86</v>
+      </c>
       <c r="I8" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J8" s="7"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>30</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="17" t="s">
-        <v>387</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="J9" s="7"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="I10" s="17" t="s">
-        <v>387</v>
-      </c>
-      <c r="J10" s="5"/>
+        <v>386</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
+        <v>117</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" t="s">
-        <v>400</v>
-      </c>
-      <c r="G11" t="s">
-        <v>401</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
       <c r="I11" s="17" t="s">
-        <v>387</v>
-      </c>
+        <v>386</v>
+      </c>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>398</v>
+      </c>
+      <c r="G12" t="s">
+        <v>399</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>138</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>36</v>
       </c>
-      <c r="H13" t="s">
-        <v>398</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
+      <c r="H14" t="s">
+        <v>396</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>161</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C15" t="s">
         <v>37</v>
       </c>
-      <c r="H14" t="s">
-        <v>399</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" t="s">
-        <v>162</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
       <c r="H15" t="s">
-        <v>163</v>
+        <v>397</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>122</v>
+        <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>162</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H16" t="s">
-        <v>398</v>
+        <v>163</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+      <c r="H18" t="s">
+        <v>400</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>139</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>43</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H19" t="s">
+        <v>400</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="B20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" t="s">
+        <v>401</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>180</v>
+      </c>
+      <c r="C21" t="s">
+        <v>45</v>
+      </c>
+      <c r="H21" t="s">
+        <v>181</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C22" t="s">
         <v>402</v>
       </c>
-      <c r="I18" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="B19" t="s">
-        <v>178</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="H19" t="s">
-        <v>403</v>
-      </c>
-      <c r="I19" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>180</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" t="s">
-        <v>181</v>
-      </c>
-      <c r="I20" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B21" t="s">
-        <v>179</v>
-      </c>
-      <c r="C21" t="s">
-        <v>404</v>
-      </c>
-      <c r="H21" t="s">
-        <v>409</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="B22" t="s">
-        <v>140</v>
-      </c>
-      <c r="C22" t="s">
-        <v>46</v>
-      </c>
       <c r="H22" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>12</v>
+        <v>202</v>
       </c>
       <c r="B23" t="s">
-        <v>204</v>
+        <v>140</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H23" t="s">
-        <v>203</v>
+        <v>403</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>204</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" t="s">
+        <v>203</v>
+      </c>
+      <c r="I24" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>141</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>48</v>
       </c>
-      <c r="H24" t="s">
-        <v>398</v>
-      </c>
-      <c r="I24" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>214</v>
-      </c>
-      <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
+      <c r="H25" t="s">
+        <v>396</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>214</v>
+      </c>
+      <c r="B26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>122</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>51</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>52</v>
       </c>
-      <c r="I26" s="17" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
+      <c r="I27" s="17" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B28" t="s">
         <v>216</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>53</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H28" t="s">
         <v>218</v>
       </c>
-      <c r="I27" s="17"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>122</v>
-      </c>
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" t="s">
-        <v>55</v>
-      </c>
-      <c r="I28" s="17" t="s">
-        <v>387</v>
-      </c>
+      <c r="I28" s="17"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>239</v>
+        <v>122</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C29" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="B30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="B31" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B32" t="s">
-        <v>375</v>
+        <v>60</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>122</v>
+        <v>267</v>
       </c>
       <c r="B33" t="s">
-        <v>63</v>
+        <v>374</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
-      </c>
-      <c r="H33" t="s">
-        <v>268</v>
+        <v>62</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>290</v>
+        <v>122</v>
       </c>
       <c r="B34" t="s">
-        <v>269</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="H34" t="s">
+        <v>268</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>308</v>
+        <v>290</v>
       </c>
       <c r="B35" t="s">
-        <v>66</v>
+        <v>269</v>
       </c>
       <c r="C35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>308</v>
       </c>
       <c r="B36" t="s">
-        <v>309</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>386</v>
-      </c>
-      <c r="H36" t="s">
-        <v>310</v>
+        <v>67</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>325</v>
+        <v>12</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>309</v>
       </c>
       <c r="C37" t="s">
-        <v>69</v>
+        <v>385</v>
+      </c>
+      <c r="H37" t="s">
+        <v>310</v>
       </c>
       <c r="I37" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>12</v>
+        <v>414</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I38" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>12</v>
       </c>
       <c r="B39" t="s">
-        <v>142</v>
+        <v>70</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I39" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>335</v>
+        <v>122</v>
       </c>
       <c r="B40" t="s">
-        <v>336</v>
+        <v>142</v>
       </c>
       <c r="C40" t="s">
-        <v>73</v>
-      </c>
-      <c r="H40" t="s">
-        <v>341</v>
+        <v>72</v>
       </c>
       <c r="I40" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="B41" t="s">
-        <v>337</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>338</v>
+        <v>335</v>
+      </c>
+      <c r="C41" t="s">
+        <v>73</v>
       </c>
       <c r="H41" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I41" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="B42" t="s">
-        <v>339</v>
-      </c>
-      <c r="C42" t="s">
+        <v>336</v>
+      </c>
+      <c r="C42" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="H42" t="s">
         <v>340</v>
       </c>
-      <c r="H42" t="s">
-        <v>341</v>
-      </c>
       <c r="I42" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>122</v>
+        <v>362</v>
       </c>
       <c r="B43" t="s">
-        <v>381</v>
+        <v>338</v>
       </c>
       <c r="C43" t="s">
-        <v>74</v>
+        <v>339</v>
       </c>
       <c r="H43" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I43" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>369</v>
+        <v>122</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>380</v>
       </c>
       <c r="C44" t="s">
-        <v>364</v>
+        <v>74</v>
+      </c>
+      <c r="H44" t="s">
+        <v>340</v>
       </c>
       <c r="I44" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="I45" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C46" t="s">
         <v>366</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B47" t="s">
-        <v>382</v>
+        <v>77</v>
       </c>
       <c r="C47" t="s">
         <v>365</v>
       </c>
       <c r="I47" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>122</v>
+        <v>368</v>
       </c>
       <c r="B48" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>364</v>
       </c>
       <c r="I48" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="C49" t="s">
-        <v>79</v>
-      </c>
-      <c r="H49" t="s">
-        <v>380</v>
+        <v>78</v>
       </c>
       <c r="I49" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B50" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>79</v>
+      </c>
+      <c r="H50" t="s">
+        <v>379</v>
       </c>
       <c r="I50" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2628,65 +2653,79 @@
         <v>122</v>
       </c>
       <c r="B51" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="C51" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I51" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>12</v>
+        <v>122</v>
       </c>
       <c r="B52" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C52" t="s">
-        <v>82</v>
-      </c>
-      <c r="H52" t="s">
-        <v>377</v>
+        <v>81</v>
       </c>
       <c r="I52" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>217</v>
-      </c>
-      <c r="I53" s="17"/>
+        <v>12</v>
+      </c>
+      <c r="B53" t="s">
+        <v>377</v>
+      </c>
+      <c r="C53" t="s">
+        <v>82</v>
+      </c>
+      <c r="H53" t="s">
+        <v>376</v>
+      </c>
+      <c r="I53" s="17" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>12</v>
-      </c>
-      <c r="B54" t="s">
-        <v>83</v>
-      </c>
-      <c r="C54" t="s">
-        <v>13</v>
-      </c>
-      <c r="I54" s="12"/>
+        <v>217</v>
+      </c>
+      <c r="I54" s="17"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>370</v>
+        <v>12</v>
       </c>
       <c r="B55" t="s">
-        <v>372</v>
+        <v>83</v>
+      </c>
+      <c r="C55" t="s">
+        <v>13</v>
       </c>
       <c r="I55" s="12"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>369</v>
+      </c>
+      <c r="B56" t="s">
         <v>371</v>
       </c>
-      <c r="B56" t="s">
-        <v>373</v>
+      <c r="I56" s="12"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>370</v>
+      </c>
+      <c r="B57" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -2697,10 +2736,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F139"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2793,7 +2832,7 @@
         <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3109,21 +3148,21 @@
         <v>158</v>
       </c>
       <c r="B36" t="s">
-        <v>115</v>
+        <v>413</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>412</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="B37" t="s">
-        <v>173</v>
+        <v>115</v>
       </c>
       <c r="C37" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3131,10 +3170,10 @@
         <v>171</v>
       </c>
       <c r="B38" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="C38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3142,10 +3181,10 @@
         <v>171</v>
       </c>
       <c r="B39" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C39" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3153,10 +3192,10 @@
         <v>171</v>
       </c>
       <c r="B40" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C40" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -3164,10 +3203,10 @@
         <v>171</v>
       </c>
       <c r="B41" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="C41" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3175,21 +3214,21 @@
         <v>171</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>153</v>
       </c>
       <c r="C42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="25" t="s">
-        <v>201</v>
+        <v>171</v>
       </c>
       <c r="B43" t="s">
-        <v>192</v>
+        <v>115</v>
       </c>
       <c r="C43" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -3197,10 +3236,10 @@
         <v>201</v>
       </c>
       <c r="B44" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C44" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -3208,10 +3247,10 @@
         <v>201</v>
       </c>
       <c r="B45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C45" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -3219,10 +3258,10 @@
         <v>201</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C46" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
@@ -3230,10 +3269,10 @@
         <v>201</v>
       </c>
       <c r="B47" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C47" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -3241,10 +3280,10 @@
         <v>201</v>
       </c>
       <c r="B48" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C48" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3252,10 +3291,10 @@
         <v>201</v>
       </c>
       <c r="B49" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C49" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -3263,10 +3302,10 @@
         <v>201</v>
       </c>
       <c r="B50" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C50" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -3274,10 +3313,10 @@
         <v>201</v>
       </c>
       <c r="B51" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C51" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3285,21 +3324,21 @@
         <v>201</v>
       </c>
       <c r="B52" t="s">
+        <v>200</v>
+      </c>
+      <c r="C52" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="B53" t="s">
         <v>115</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>191</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="27" t="s">
-        <v>213</v>
-      </c>
-      <c r="B53" t="s">
-        <v>209</v>
-      </c>
-      <c r="C53" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3307,10 +3346,10 @@
         <v>213</v>
       </c>
       <c r="B54" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C54" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -3318,10 +3357,10 @@
         <v>213</v>
       </c>
       <c r="B55" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C55" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -3329,21 +3368,21 @@
         <v>213</v>
       </c>
       <c r="B56" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C56" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="27" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
       <c r="B57" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C57" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -3351,10 +3390,10 @@
         <v>238</v>
       </c>
       <c r="B58" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C58" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -3362,10 +3401,10 @@
         <v>238</v>
       </c>
       <c r="B59" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="C59" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
@@ -3373,10 +3412,10 @@
         <v>238</v>
       </c>
       <c r="B60" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C60" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
@@ -3384,10 +3423,10 @@
         <v>238</v>
       </c>
       <c r="B61" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C61" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -3395,10 +3434,10 @@
         <v>238</v>
       </c>
       <c r="B62" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C62" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -3406,10 +3445,10 @@
         <v>238</v>
       </c>
       <c r="B63" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C63" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -3417,10 +3456,10 @@
         <v>238</v>
       </c>
       <c r="B64" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="C64" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -3428,10 +3467,10 @@
         <v>238</v>
       </c>
       <c r="B65" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C65" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
@@ -3439,10 +3478,10 @@
         <v>238</v>
       </c>
       <c r="B66" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C66" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
@@ -3450,10 +3489,10 @@
         <v>238</v>
       </c>
       <c r="B67" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C67" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
@@ -3461,21 +3500,21 @@
         <v>238</v>
       </c>
       <c r="B68" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="C68" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="27" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B69" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C69" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
@@ -3483,10 +3522,10 @@
         <v>245</v>
       </c>
       <c r="B70" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
       <c r="C70" t="s">
-        <v>220</v>
+        <v>240</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
@@ -3494,10 +3533,10 @@
         <v>245</v>
       </c>
       <c r="B71" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="C71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
@@ -3505,10 +3544,10 @@
         <v>245</v>
       </c>
       <c r="B72" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C72" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
@@ -3516,10 +3555,10 @@
         <v>245</v>
       </c>
       <c r="B73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C73" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
@@ -3527,10 +3566,10 @@
         <v>245</v>
       </c>
       <c r="B74" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C74" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
@@ -3538,10 +3577,10 @@
         <v>245</v>
       </c>
       <c r="B75" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="C75" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
@@ -3549,10 +3588,10 @@
         <v>245</v>
       </c>
       <c r="B76" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="C76" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
@@ -3560,10 +3599,10 @@
         <v>245</v>
       </c>
       <c r="B77" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C77" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
@@ -3571,10 +3610,10 @@
         <v>245</v>
       </c>
       <c r="B78" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C78" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
@@ -3582,10 +3621,10 @@
         <v>245</v>
       </c>
       <c r="B79" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C79" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
@@ -3593,10 +3632,10 @@
         <v>245</v>
       </c>
       <c r="B80" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="C80" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -3604,21 +3643,21 @@
         <v>245</v>
       </c>
       <c r="B81" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C81" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="27" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="B82" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C82" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
@@ -3626,10 +3665,10 @@
         <v>256</v>
       </c>
       <c r="B83" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C83" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
@@ -3637,10 +3676,10 @@
         <v>256</v>
       </c>
       <c r="B84" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="C84" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
@@ -3648,10 +3687,10 @@
         <v>256</v>
       </c>
       <c r="B85" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="C85" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -3659,21 +3698,21 @@
         <v>256</v>
       </c>
       <c r="B86" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C86" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="27" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="B87" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C87" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -3681,10 +3720,10 @@
         <v>266</v>
       </c>
       <c r="B88" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C88" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -3692,10 +3731,10 @@
         <v>266</v>
       </c>
       <c r="B89" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C89" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -3703,21 +3742,21 @@
         <v>266</v>
       </c>
       <c r="B90" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C90" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="27" t="s">
-        <v>289</v>
+        <v>266</v>
       </c>
       <c r="B91" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C91" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -3725,10 +3764,10 @@
         <v>289</v>
       </c>
       <c r="B92" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C92" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -3736,10 +3775,10 @@
         <v>289</v>
       </c>
       <c r="B93" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C93" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -3747,10 +3786,10 @@
         <v>289</v>
       </c>
       <c r="B94" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C94" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -3758,10 +3797,10 @@
         <v>289</v>
       </c>
       <c r="B95" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C95" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -3769,10 +3808,10 @@
         <v>289</v>
       </c>
       <c r="B96" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C96" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -3780,10 +3819,10 @@
         <v>289</v>
       </c>
       <c r="B97" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C97" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -3791,10 +3830,10 @@
         <v>289</v>
       </c>
       <c r="B98" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C98" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -3802,10 +3841,10 @@
         <v>289</v>
       </c>
       <c r="B99" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C99" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -3813,21 +3852,21 @@
         <v>289</v>
       </c>
       <c r="B100" t="s">
-        <v>115</v>
+        <v>288</v>
       </c>
       <c r="C100" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="27" t="s">
-        <v>307</v>
+        <v>289</v>
       </c>
       <c r="B101" t="s">
-        <v>300</v>
+        <v>115</v>
       </c>
       <c r="C101" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -3835,10 +3874,10 @@
         <v>307</v>
       </c>
       <c r="B102" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C102" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -3846,10 +3885,10 @@
         <v>307</v>
       </c>
       <c r="B103" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C103" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -3857,10 +3896,10 @@
         <v>307</v>
       </c>
       <c r="B104" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C104" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
@@ -3868,10 +3907,10 @@
         <v>307</v>
       </c>
       <c r="B105" t="s">
-        <v>295</v>
+        <v>303</v>
       </c>
       <c r="C105" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
@@ -3879,10 +3918,10 @@
         <v>307</v>
       </c>
       <c r="B106" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C106" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
@@ -3890,10 +3929,10 @@
         <v>307</v>
       </c>
       <c r="B107" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C107" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
@@ -3901,10 +3940,10 @@
         <v>307</v>
       </c>
       <c r="B108" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C108" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -3912,21 +3951,21 @@
         <v>307</v>
       </c>
       <c r="B109" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="C109" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="27" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
       <c r="B110" t="s">
-        <v>318</v>
+        <v>299</v>
       </c>
       <c r="C110" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -3934,10 +3973,10 @@
         <v>324</v>
       </c>
       <c r="B111" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C111" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3945,10 +3984,10 @@
         <v>324</v>
       </c>
       <c r="B112" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C112" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -3956,10 +3995,10 @@
         <v>324</v>
       </c>
       <c r="B113" t="s">
-        <v>303</v>
+        <v>320</v>
       </c>
       <c r="C113" t="s">
-        <v>294</v>
+        <v>313</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -3967,10 +4006,10 @@
         <v>324</v>
       </c>
       <c r="B114" t="s">
-        <v>321</v>
+        <v>303</v>
       </c>
       <c r="C114" t="s">
-        <v>314</v>
+        <v>294</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -3978,10 +4017,10 @@
         <v>324</v>
       </c>
       <c r="B115" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C115" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
@@ -3989,10 +4028,10 @@
         <v>324</v>
       </c>
       <c r="B116" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C116" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
@@ -4000,252 +4039,263 @@
         <v>324</v>
       </c>
       <c r="B117" t="s">
-        <v>317</v>
+        <v>323</v>
       </c>
       <c r="C117" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="27" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
       <c r="B118" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="C118" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B119" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C119" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B120" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C120" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="27" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B121" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C121" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="27" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="B122" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C122" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B123" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C123" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B124" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C124" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B125" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C125" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="27" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B126" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="C126" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="27" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
       <c r="B127" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="C127" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B128" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C128" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B129" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C129" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="27" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B130" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C130" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="27" t="s">
-        <v>368</v>
-      </c>
-      <c r="B131">
-        <v>1</v>
-      </c>
-      <c r="C131">
-        <v>1</v>
+        <v>361</v>
+      </c>
+      <c r="B131" t="s">
+        <v>360</v>
+      </c>
+      <c r="C131" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B132">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C132">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B133">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C133">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B134">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C134">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B135">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C135">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B136">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C136">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="27" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B137">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C137">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="27" t="s">
-        <v>388</v>
-      </c>
-      <c r="B138" t="s">
-        <v>391</v>
-      </c>
-      <c r="C138" t="s">
-        <v>389</v>
+        <v>367</v>
+      </c>
+      <c r="B138">
+        <v>7</v>
+      </c>
+      <c r="C138">
+        <v>7</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="27" t="s">
+        <v>387</v>
+      </c>
+      <c r="B139" t="s">
+        <v>390</v>
+      </c>
+      <c r="C139" t="s">
         <v>388</v>
       </c>
-      <c r="B139" t="s">
-        <v>392</v>
-      </c>
-      <c r="C139" t="s">
-        <v>390</v>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="27" t="s">
+        <v>387</v>
+      </c>
+      <c r="B140" t="s">
+        <v>391</v>
+      </c>
+      <c r="C140" t="s">
+        <v>389</v>
       </c>
     </row>
   </sheetData>
@@ -4286,10 +4336,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="B2" t="s">
         <v>406</v>
-      </c>
-      <c r="B2" t="s">
-        <v>408</v>
       </c>
       <c r="C2" s="15">
         <v>20200305</v>

</xml_diff>